<commit_message>
start read func and add notebook
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rad/Desktop/UNi/proj/EER/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F321960A-31E0-4547-BFD4-D8ECD4B832C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63C9475-6E33-F941-9DBE-744721F603AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{170F6588-63A9-784C-A376-C92C81798569}"/>
   </bookViews>
@@ -82,7 +82,7 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://entrepreneurship.ubc.ca/</t>
+    <t>https://entrepreneurship.ubc.ca/ | https://entrepreneurship.ubc.ca/who-we-are</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7425A2F6-E9BC-3B4F-96F4-66F7380AD1FA}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{491E056C-0073-0B4C-979C-A4C618C64A92}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{C866142E-86E3-F943-B40D-24A8E7E5C311}"/>
+    <hyperlink ref="B2" r:id="rId3" display="https://entrepreneurship.ubc.ca/" xr:uid="{C866142E-86E3-F943-B40D-24A8E7E5C311}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>